<commit_message>
excelJs module made according to the template
</commit_message>
<xml_diff>
--- a/final-template.xlsx
+++ b/final-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/staff/test-xlsx-export-libraries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149B6AFC-858B-4543-BAD6-98E63539B474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182E27D8-7884-6C43-818F-AFB9EE3161EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="27580" windowHeight="17100" activeTab="1" xr2:uid="{6DB4F2E6-2AD1-6549-9B7B-08E0F3A1BD6C}"/>
   </bookViews>
@@ -16,7 +16,10 @@
     <sheet name="Красивый лист" sheetId="1" r:id="rId1"/>
     <sheet name="Другой лист" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Другой лист'!$A$1:$E$5</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -582,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129743B4-B4DB-BB4F-8B64-B969BECDB3CB}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,6 +598,7 @@
     <col min="4" max="4" width="39.5" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
@@ -676,6 +680,9 @@
       <c r="F4" s="4">
         <v>1234</v>
       </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -687,7 +694,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -696,7 +703,7 @@
     <col min="2" max="2" width="23.5" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="56.83203125" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" customWidth="1"/>
     <col min="6" max="6" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -837,6 +844,10 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E5" xr:uid="{DC13381C-53A2-0543-BF1B-D57B2F36E09A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E5">
+    <sortCondition descending="1" ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>